<commit_message>
0.4.1 : Update version
</commit_message>
<xml_diff>
--- a/templates/template_0.4.1.xlsx
+++ b/templates/template_0.4.1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxime\Documents\SwissClimate\BuildingsEmissionsCalculator\CorruptedFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxime\Documents\SwissClimate\BuildingsEmissionsCalculator\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8678DEB-2864-4B34-B88C-995A46ED935A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2071CBE1-8F39-437F-87DC-9D4CDCB06F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="156">
   <si>
     <t>Identification du batiment</t>
   </si>
@@ -600,30 +600,12 @@
     <t>Nom et Numéro de rue sur la même ligne</t>
   </si>
   <si>
-    <t>tot_mortgage_emissions</t>
-  </si>
-  <si>
-    <t>tot_asset_energetic_area</t>
-  </si>
-  <si>
-    <t>tot_asset_emissions</t>
-  </si>
-  <si>
-    <t>mean_emissions_per_area</t>
-  </si>
-  <si>
     <t>Total emissions of the assets (in kg CO2)</t>
   </si>
   <si>
     <t>Total Surface of the assets (m2)</t>
   </si>
   <si>
-    <t>tot_mortgage_value</t>
-  </si>
-  <si>
-    <t>count_mortgage</t>
-  </si>
-  <si>
     <t>Coverage (in number of mortgages found)</t>
   </si>
   <si>
@@ -639,35 +621,26 @@
     <t>Mortgage amount under consideration without missing data (CHF)</t>
   </si>
   <si>
-    <t>tot_mortgage_value_found</t>
-  </si>
-  <si>
     <t>Number of Missing Mortgages Emission</t>
   </si>
   <si>
-    <t>count_mortgage_emissions_not_found</t>
-  </si>
-  <si>
-    <t>coverage_mortgage_emissions_count</t>
-  </si>
-  <si>
-    <t>coverage_mortgage_emissions_value</t>
-  </si>
-  <si>
-    <t>mean_missions_intensity</t>
-  </si>
-  <si>
     <t>Template Version</t>
   </si>
   <si>
     <t>0.4.1</t>
+  </si>
+  <si>
+    <t>Not working now ! -&gt; Les cases vides ne sont pas considérées comme vide par Excel. TODO: Trouver pourquoi</t>
+  </si>
+  <si>
+    <t>Not working now !</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -725,8 +698,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -781,8 +761,14 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="38">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1313,11 +1299,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1449,6 +1444,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="8" fillId="10" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="8" fillId="10" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="10" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1606,48 +1605,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5D874FD6-80FA-4D98-BF8F-BB7152598394}" name="summary_table" displayName="summary_table" ref="B4:L5" totalsRowShown="0">
-  <autoFilter ref="B4:L5" xr:uid="{5D874FD6-80FA-4D98-BF8F-BB7152598394}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EBAD434D-D871-4EDD-A3DE-A8797628D847}" name="tot_asset_energetic_area">
-      <calculatedColumnFormula>SUM(buildings_table[asset_energetic_area])</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" xr3:uid="{8C4F42E9-3C1E-4FF5-84FA-37711AA14AB5}" name="tot_asset_emissions">
-      <calculatedColumnFormula>SUM(buildings_table[asset_emissions])</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{9B95790F-45CC-4622-881C-EE0F53C168B9}" name="tot_mortgage_emissions">
-      <calculatedColumnFormula>SUM(buildings_table[mortgage_emissions])</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="4" xr3:uid="{258C1E9F-FFAC-4FEC-8FB3-08384FE62842}" name="mean_missions_intensity">
-      <calculatedColumnFormula>summary_table[[#This Row],[tot_mortgage_emissions]]/summary_table[[#This Row],[tot_mortgage_value_found]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{43AD4D65-2020-411F-A6E7-9EC7D9822320}" name="mean_emissions_per_area">
-      <calculatedColumnFormula>AVERAGE(buildings_table[emissions_per_area])</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{3395B87A-75FA-435C-929D-23F82AEEF073}" name="tot_mortgage_value">
-      <calculatedColumnFormula>SUM(buildings_table[mortgage_value])</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{B3D23EF3-9BFE-4A09-8CF1-AADB0BE9913F}" name="tot_mortgage_value_found">
-      <calculatedColumnFormula>SUMIFS(buildings_table[mortgage_value], buildings_table[mortgage_emissions], "&lt;&gt;")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{93AD0051-42A2-4057-91B0-C31518276D31}" name="count_mortgage">
-      <calculatedColumnFormula>ROWS(buildings_table[mortgage_emissions])</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{B362F588-95F3-41D5-B378-2EF6DCE8F863}" name="count_mortgage_emissions_not_found">
-      <calculatedColumnFormula>COUNTBLANK(buildings_table[mortgage_emissions])</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{D7356970-F441-4CD3-AB5B-35CCC6B04F8A}" name="coverage_mortgage_emissions_count">
-      <calculatedColumnFormula>(COUNTA(buildings_table[mortgage_emissions])/ROWS(buildings_table[mortgage_emissions]))</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="11" xr3:uid="{A668BEB9-BA06-4F76-B11C-DEB8210DDBF2}" name="coverage_mortgage_emissions_value">
-      <calculatedColumnFormula>summary_table[[#This Row],[tot_mortgage_value_found]]/summary_table[[#This Row],[tot_mortgage_value]]</calculatedColumnFormula>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="buildings_table" displayName="buildings_table" ref="B5:AU6" insertRow="1" totalsRowShown="0">
   <autoFilter ref="B5:AU6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="46">
@@ -1989,15 +1946,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="62.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.140625" bestFit="1" customWidth="1"/>
@@ -2011,142 +1968,122 @@
     <col min="12" max="12" width="48.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B1" t="s">
-        <v>164</v>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="J3" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="K3" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="L3" s="27" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="C4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H4" t="s">
-        <v>157</v>
-      </c>
-      <c r="I4" t="s">
-        <v>151</v>
-      </c>
-      <c r="J4" t="s">
-        <v>159</v>
-      </c>
-      <c r="K4" t="s">
-        <v>160</v>
-      </c>
-      <c r="L4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5">
+      <c r="B3" s="48">
         <f>SUM(buildings_table[asset_energetic_area])</f>
         <v>0</v>
       </c>
-      <c r="C5">
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="48">
         <f>SUM(buildings_table[asset_emissions])</f>
         <v>0</v>
       </c>
-      <c r="D5">
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="48">
         <f>SUM(buildings_table[mortgage_emissions])</f>
         <v>0</v>
       </c>
-      <c r="E5" t="e">
-        <f>summary_table[[#This Row],[tot_mortgage_emissions]]/summary_table[[#This Row],[tot_mortgage_value_found]]</f>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="48" t="e">
+        <f>B5/B9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F5" t="e">
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="48" t="e">
         <f>AVERAGE(buildings_table[emissions_per_area])</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="G5" s="40">
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="48">
         <f>SUM(buildings_table[mortgage_value])</f>
         <v>0</v>
       </c>
-      <c r="H5">
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="48">
         <f>SUMIFS(buildings_table[mortgage_value], buildings_table[mortgage_emissions], "&lt;&gt;")</f>
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="C9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="49">
         <f>ROWS(buildings_table[mortgage_emissions])</f>
         <v>1</v>
       </c>
-      <c r="J5">
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="49">
         <f>COUNTBLANK(buildings_table[mortgage_emissions])</f>
         <v>1</v>
       </c>
-      <c r="K5">
-        <f>(COUNTA(buildings_table[mortgage_emissions])/ROWS(buildings_table[mortgage_emissions]))</f>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="50">
+        <f>1-B11/B10</f>
         <v>0</v>
       </c>
-      <c r="L5" t="e">
-        <f>summary_table[[#This Row],[tot_mortgage_value_found]]/summary_table[[#This Row],[tot_mortgage_value]]</f>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="50" t="e">
+        <f>B9/B8</f>
         <v>#DIV/0!</v>
+      </c>
+      <c r="C13" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -2211,61 +2148,61 @@
   <sheetData>
     <row r="1" spans="1:47" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="52" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="49" t="s">
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="50"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="54" t="s">
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
-      <c r="AH1" s="55"/>
-      <c r="AI1" s="55"/>
-      <c r="AJ1" s="55"/>
-      <c r="AK1" s="55"/>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="55"/>
-      <c r="AN1" s="56"/>
-      <c r="AO1" s="53" t="s">
+      <c r="AE1" s="59"/>
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="59"/>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="59"/>
+      <c r="AK1" s="59"/>
+      <c r="AL1" s="59"/>
+      <c r="AM1" s="59"/>
+      <c r="AN1" s="60"/>
+      <c r="AO1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="AP1" s="53"/>
-      <c r="AQ1" s="53"/>
-      <c r="AR1" s="53"/>
-      <c r="AS1" s="53"/>
-      <c r="AT1" s="53"/>
+      <c r="AP1" s="57"/>
+      <c r="AQ1" s="57"/>
+      <c r="AR1" s="57"/>
+      <c r="AS1" s="57"/>
+      <c r="AT1" s="57"/>
       <c r="AU1" s="39" t="s">
         <v>4</v>
       </c>
@@ -2855,26 +2792,26 @@
     <row r="1" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="59"/>
-      <c r="I1" s="60" t="s">
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="63"/>
+      <c r="I1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="62"/>
-      <c r="P1" s="63" t="s">
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="66"/>
+      <c r="P1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="65"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="69"/>
       <c r="T1" s="20" t="s">
         <v>4</v>
       </c>

</xml_diff>